<commit_message>
Intermediate Update [26/05] Logging delays, ensembles, TW's and more
</commit_message>
<xml_diff>
--- a/upload/runs/1 min/1 min ADH931_.xlsx
+++ b/upload/runs/1 min/1 min ADH931_.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Git 2\upload\runs\1 min\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB29403F-DC56-475D-AABC-DA70332A59DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4740" yWindow="1620" windowWidth="24060" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1768,8 +1774,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1832,6 +1838,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1878,7 +1892,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1910,9 +1924,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1944,6 +1976,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2119,14 +2169,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2349,7 +2402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2369,7 +2422,7 @@
         <v>40</v>
       </c>
       <c r="G3">
-        <v>2305.171</v>
+        <v>2305.1709999999998</v>
       </c>
       <c r="H3" t="s">
         <v>38</v>
@@ -2462,7 +2515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2482,7 +2535,7 @@
         <v>41</v>
       </c>
       <c r="G4">
-        <v>2559.582</v>
+        <v>2559.5819999999999</v>
       </c>
       <c r="H4" t="s">
         <v>38</v>
@@ -2575,7 +2628,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2595,7 +2648,7 @@
         <v>42</v>
       </c>
       <c r="G5">
-        <v>2458.978</v>
+        <v>2458.9780000000001</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -2688,7 +2741,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2708,7 +2761,7 @@
         <v>43</v>
       </c>
       <c r="G6">
-        <v>2314.8</v>
+        <v>2314.8000000000002</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -2801,7 +2854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2821,7 +2874,7 @@
         <v>44</v>
       </c>
       <c r="G7">
-        <v>2543.822</v>
+        <v>2543.8220000000001</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -2914,7 +2967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2934,7 +2987,7 @@
         <v>41</v>
       </c>
       <c r="G8">
-        <v>2537.485</v>
+        <v>2537.4850000000001</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
@@ -3027,7 +3080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3047,7 +3100,7 @@
         <v>43</v>
       </c>
       <c r="G9">
-        <v>2444.766</v>
+        <v>2444.7660000000001</v>
       </c>
       <c r="H9" t="s">
         <v>38</v>
@@ -3140,7 +3193,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3160,7 +3213,7 @@
         <v>40</v>
       </c>
       <c r="G10">
-        <v>2401.678</v>
+        <v>2401.6779999999999</v>
       </c>
       <c r="H10" t="s">
         <v>38</v>
@@ -3253,7 +3306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3273,7 +3326,7 @@
         <v>45</v>
       </c>
       <c r="G11">
-        <v>2471.324</v>
+        <v>2471.3240000000001</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
@@ -3366,7 +3419,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3479,7 +3532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3499,7 +3552,7 @@
         <v>46</v>
       </c>
       <c r="G13">
-        <v>2293.865</v>
+        <v>2293.8649999999998</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -3592,7 +3645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3612,7 +3665,7 @@
         <v>47</v>
       </c>
       <c r="G14">
-        <v>2306.426</v>
+        <v>2306.4259999999999</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -3705,7 +3758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3725,7 +3778,7 @@
         <v>48</v>
       </c>
       <c r="G15">
-        <v>2324.146</v>
+        <v>2324.1460000000002</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -3818,7 +3871,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3931,7 +3984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3951,7 +4004,7 @@
         <v>50</v>
       </c>
       <c r="G17">
-        <v>2540.378</v>
+        <v>2540.3780000000002</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>
@@ -4044,7 +4097,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4064,7 +4117,7 @@
         <v>51</v>
       </c>
       <c r="G18">
-        <v>2543.492</v>
+        <v>2543.4920000000002</v>
       </c>
       <c r="H18" t="s">
         <v>38</v>
@@ -4157,7 +4210,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4177,7 +4230,7 @@
         <v>52</v>
       </c>
       <c r="G19">
-        <v>2323.501</v>
+        <v>2323.5010000000002</v>
       </c>
       <c r="H19" t="s">
         <v>38</v>
@@ -4270,7 +4323,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4290,7 +4343,7 @@
         <v>53</v>
       </c>
       <c r="G20">
-        <v>2452.016</v>
+        <v>2452.0160000000001</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
@@ -4383,7 +4436,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4403,7 +4456,7 @@
         <v>48</v>
       </c>
       <c r="G21">
-        <v>2536.675</v>
+        <v>2536.6750000000002</v>
       </c>
       <c r="H21" t="s">
         <v>38</v>
@@ -4496,7 +4549,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4516,7 +4569,7 @@
         <v>43</v>
       </c>
       <c r="G22">
-        <v>2406.794</v>
+        <v>2406.7939999999999</v>
       </c>
       <c r="H22" t="s">
         <v>38</v>
@@ -4609,7 +4662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4722,7 +4775,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4742,7 +4795,7 @@
         <v>52</v>
       </c>
       <c r="G24">
-        <v>2411.941</v>
+        <v>2411.9409999999998</v>
       </c>
       <c r="H24" t="s">
         <v>38</v>
@@ -4835,7 +4888,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4948,7 +5001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4968,7 +5021,7 @@
         <v>47</v>
       </c>
       <c r="G26">
-        <v>2407.572</v>
+        <v>2407.5720000000001</v>
       </c>
       <c r="H26" t="s">
         <v>38</v>
@@ -5061,7 +5114,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5174,7 +5227,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5287,7 +5340,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5307,7 +5360,7 @@
         <v>43</v>
       </c>
       <c r="G29">
-        <v>2450.919</v>
+        <v>2450.9189999999999</v>
       </c>
       <c r="H29" t="s">
         <v>38</v>
@@ -5400,7 +5453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5513,7 +5566,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5533,7 +5586,7 @@
         <v>41</v>
       </c>
       <c r="G31">
-        <v>2448.594</v>
+        <v>2448.5940000000001</v>
       </c>
       <c r="H31" t="s">
         <v>38</v>
@@ -5626,7 +5679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5646,7 +5699,7 @@
         <v>43</v>
       </c>
       <c r="G32">
-        <v>2409.438</v>
+        <v>2409.4380000000001</v>
       </c>
       <c r="H32" t="s">
         <v>38</v>
@@ -5739,7 +5792,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5759,7 +5812,7 @@
         <v>43</v>
       </c>
       <c r="G33">
-        <v>2463.755</v>
+        <v>2463.7550000000001</v>
       </c>
       <c r="H33" t="s">
         <v>38</v>
@@ -5852,7 +5905,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5872,7 +5925,7 @@
         <v>44</v>
       </c>
       <c r="G34">
-        <v>2536.458</v>
+        <v>2536.4580000000001</v>
       </c>
       <c r="H34" t="s">
         <v>38</v>
@@ -5965,7 +6018,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5985,7 +6038,7 @@
         <v>48</v>
       </c>
       <c r="G35">
-        <v>2400.832</v>
+        <v>2400.8319999999999</v>
       </c>
       <c r="H35" t="s">
         <v>38</v>
@@ -6078,7 +6131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -6098,7 +6151,7 @@
         <v>40</v>
       </c>
       <c r="G36">
-        <v>2405.702</v>
+        <v>2405.7020000000002</v>
       </c>
       <c r="H36" t="s">
         <v>38</v>
@@ -6191,7 +6244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -6304,7 +6357,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -6324,7 +6377,7 @@
         <v>40</v>
       </c>
       <c r="G38">
-        <v>2408.315</v>
+        <v>2408.3150000000001</v>
       </c>
       <c r="H38" t="s">
         <v>38</v>
@@ -6417,7 +6470,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6437,7 +6490,7 @@
         <v>40</v>
       </c>
       <c r="G39">
-        <v>2217.427</v>
+        <v>2217.4270000000001</v>
       </c>
       <c r="H39" t="s">
         <v>38</v>
@@ -6530,7 +6583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6550,7 +6603,7 @@
         <v>53</v>
       </c>
       <c r="G40">
-        <v>2541.175</v>
+        <v>2541.1750000000002</v>
       </c>
       <c r="H40" t="s">
         <v>38</v>
@@ -6643,7 +6696,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6663,7 +6716,7 @@
         <v>40</v>
       </c>
       <c r="G41">
-        <v>2427.423</v>
+        <v>2427.4229999999998</v>
       </c>
       <c r="H41" t="s">
         <v>38</v>
@@ -6756,7 +6809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6776,7 +6829,7 @@
         <v>55</v>
       </c>
       <c r="G42">
-        <v>2384.847</v>
+        <v>2384.8470000000002</v>
       </c>
       <c r="H42" t="s">
         <v>38</v>
@@ -6869,7 +6922,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6889,7 +6942,7 @@
         <v>48</v>
       </c>
       <c r="G43">
-        <v>2440.276</v>
+        <v>2440.2759999999998</v>
       </c>
       <c r="H43" t="s">
         <v>38</v>
@@ -6982,7 +7035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -7095,7 +7148,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -7208,7 +7261,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -7228,7 +7281,7 @@
         <v>54</v>
       </c>
       <c r="G46">
-        <v>2408.24</v>
+        <v>2408.2399999999998</v>
       </c>
       <c r="H46" t="s">
         <v>38</v>
@@ -7321,7 +7374,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -7341,7 +7394,7 @@
         <v>43</v>
       </c>
       <c r="G47">
-        <v>2316.679</v>
+        <v>2316.6790000000001</v>
       </c>
       <c r="H47" t="s">
         <v>38</v>
@@ -7434,7 +7487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -7454,7 +7507,7 @@
         <v>40</v>
       </c>
       <c r="G48">
-        <v>2401.428</v>
+        <v>2401.4279999999999</v>
       </c>
       <c r="H48" t="s">
         <v>38</v>
@@ -7547,7 +7600,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -7567,7 +7620,7 @@
         <v>44</v>
       </c>
       <c r="G49">
-        <v>2401.613</v>
+        <v>2401.6129999999998</v>
       </c>
       <c r="H49" t="s">
         <v>38</v>
@@ -7660,7 +7713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -7680,7 +7733,7 @@
         <v>43</v>
       </c>
       <c r="G50">
-        <v>2430.469</v>
+        <v>2430.4690000000001</v>
       </c>
       <c r="H50" t="s">
         <v>38</v>
@@ -7773,7 +7826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -7793,7 +7846,7 @@
         <v>43</v>
       </c>
       <c r="G51">
-        <v>2533.464</v>
+        <v>2533.4639999999999</v>
       </c>
       <c r="H51" t="s">
         <v>38</v>

</xml_diff>